<commit_message>
integracao das telas com o python e ajuste do banco de dados
</commit_message>
<xml_diff>
--- a/src/base/dados_login.xlsx
+++ b/src/base/dados_login.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,32 +441,42 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>E-mail</t>
+          <t>Nome</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Nome</t>
+          <t>CPF</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CPF</t>
+          <t>Data de Nascimento</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Data de Nascimento</t>
+          <t>Senha</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Senha</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>autorizado?</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>is_active</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>is_authenticated</t>
         </is>
       </c>
     </row>
@@ -474,31 +484,70 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>matheus</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>48767507859</t>
-        </is>
+      <c r="C2" t="n">
+        <v>48767507859</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4041998</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>04041998</t>
+          <t>pbkdf2:sha256:260000$FGVLB4z6awWJ2J7w$59be00fdf0984a3c0e0949d2b2846f8d0841e9d9e49de23dc2bfdfb39edda56c</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>pbkdf2:sha256:260000$FGVLB4z6awWJ2J7w$59be00fdf0984a3c0e0949d2b2846f8d0841e9d9e49de23dc2bfdfb39edda56c</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
           <t>matheus@ufabc.edu.br</t>
         </is>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1234</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1234</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>pbkdf2:sha256:260000$5N0ofPnhoaIMtYtN$9a87a52797e5d0c6b0676b56e6e2888432a9940ebeee7a299824aac91ea32545</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>teste@ufabc.com.br</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>